<commit_message>
updating measurements and new pictures
</commit_message>
<xml_diff>
--- a/measurements.xlsx
+++ b/measurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego.garber\source\repos\MapperSpeedTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA26FEF-A428-4E5B-88E9-FCEEC67249DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86861EF-E0EE-4101-A16A-3BE6F6E905C3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1686,6 +1686,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1629283264"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
@@ -1700,6 +1701,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1337570912"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3847,8 +3849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4770,7 +4772,7 @@
         <v>6</v>
       </c>
       <c r="F38">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G38" t="s">
         <v>33</v>

</xml_diff>